<commit_message>
add test for new group parser
</commit_message>
<xml_diff>
--- a/bio_diversity/static/test/parser_test_files/test-generic-group.xlsx
+++ b/bio_diversity/static/test/parser_test_files/test-generic-group.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14565" windowHeight="5955" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14565" windowHeight="5955" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
     <sheet name="Untagged" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
+    <sheet name="Group" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,8 +25,136 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+    <author>Stoyel, Quentin</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 1999</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. Jan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>eg. Bonell</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Eg. 1999 BSR</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in to record current container, or if movement occurred.  Leave blank if movement origin is unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fill in if a movement occurred, or if origin tank is unknown.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J3" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Did the group get split, or did it move as a whole?</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>PIT</t>
   </si>
@@ -103,19 +231,16 @@
     <t>SP7</t>
   </si>
   <si>
-    <t>Skinny</t>
-  </si>
-  <si>
-    <t>Parr Marks</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
-    <t>F</t>
+    <t>Number of Fish</t>
+  </si>
+  <si>
+    <t>Whole group (Y/N)</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -125,7 +250,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +284,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -174,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -191,13 +322,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -207,6 +349,15 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -919,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:Q9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1023,7 +1174,7 @@
         <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="K4" s="3">
         <v>25</v>
@@ -1109,191 +1260,103 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:Q5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+    </row>
+    <row r="3" spans="1:12" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B1">
+      <c r="C3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
         <v>2021</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="2">
+      <c r="C4" s="2">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" t="s">
+      <c r="E4" s="1"/>
+      <c r="F4" t="s">
         <v>21</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G4" t="s">
         <v>22</v>
       </c>
-      <c r="I1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K1" s="3">
-        <v>26.1</v>
-      </c>
-      <c r="L1" s="3">
-        <v>350</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>2021</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1"/>
-      <c r="G2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2">
-        <v>27.2</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>4</v>
-      </c>
-      <c r="B3">
-        <v>2021</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="K3" s="3">
-        <v>28.3</v>
-      </c>
-      <c r="N3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>2021</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="1"/>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3">
-        <v>25.1</v>
-      </c>
-      <c r="O4">
-        <v>8</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>6</v>
-      </c>
-      <c r="B5">
-        <v>2021</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
+      <c r="J4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D5" s="2"/>
+      <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I5" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="3">
-        <v>24.3</v>
-      </c>
-      <c r="P5" t="s">
-        <v>27</v>
-      </c>
+      <c r="K5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update comment format for generic template
</commit_message>
<xml_diff>
--- a/bio_diversity/static/test/parser_test_files/test-generic-group.xlsx
+++ b/bio_diversity/static/test/parser_test_files/test-generic-group.xlsx
@@ -1,160 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stoyelq\Desktop\Work\dm_apps\dm_apps\bio_diversity\static\test\parser_test_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{302FD6B1-7A61-41ED-9854-E0D836F10578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14565" windowHeight="5955" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Individual" sheetId="3" r:id="rId1"/>
     <sheet name="Untagged" sheetId="4" r:id="rId2"/>
     <sheet name="Group" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Author</author>
-    <author>Stoyel, Quentin</author>
-  </authors>
-  <commentList>
-    <comment ref="A3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>eg. 1999</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>eg. Jan</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>eg. 1</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>eg. BSR</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E3" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>eg. Bonell</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Eg. 1999 BSR</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Fill in to record current container, or if movement occurred.  Leave blank if movement origin is unknown.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Fill in if a movement occurred, or if origin tank is unknown.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="L3" authorId="1" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Did the group get split, or did it move as a whole?</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="63">
   <si>
     <t>PIT</t>
   </si>
@@ -253,12 +135,102 @@
   </si>
   <si>
     <t>Smolt</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Vaccinated</t>
+  </si>
+  <si>
+    <t>Mark Applied</t>
+  </si>
+  <si>
+    <t>ADDITIONAL COLUMNS</t>
+  </si>
+  <si>
+    <t>eg. 1999</t>
+  </si>
+  <si>
+    <t>eg, Apr, Sep</t>
+  </si>
+  <si>
+    <t>eg. 1</t>
+  </si>
+  <si>
+    <t>Pit tag as in database</t>
+  </si>
+  <si>
+    <t>Fill in to record current container, or if movement occurred.  Leave blank if movement origin is unknown.</t>
+  </si>
+  <si>
+    <t>Fill in if a movement occurred, or if origin tank is unknown.</t>
+  </si>
+  <si>
+    <t>eg. M/F/I</t>
+  </si>
+  <si>
+    <t>Units can be set in header to (cm) or (mm), optional</t>
+  </si>
+  <si>
+    <t>Units can be set in header to (g) or (kg), optional</t>
+  </si>
+  <si>
+    <t>Vial Number, optional</t>
+  </si>
+  <si>
+    <t>Use full name Eg. Fry/Parr/Smolt. Optional</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>Scale Envelope Number, optional</t>
+  </si>
+  <si>
+    <t>Release / Keep, optional</t>
+  </si>
+  <si>
+    <t>Entry must match to Animal Detail Subjective Code in database. Optional</t>
+  </si>
+  <si>
+    <t>Enter extra columns selected in application here. Optional</t>
+  </si>
+  <si>
+    <t>UFID</t>
+  </si>
+  <si>
+    <t>Sample number, every row should be unique</t>
+  </si>
+  <si>
+    <t>Eg. SJR, TOB, STW</t>
+  </si>
+  <si>
+    <t>Eg. Bonell. Optional</t>
+  </si>
+  <si>
+    <t>Eg. Adipose Clip. Must match code in database. Optional</t>
+  </si>
+  <si>
+    <t>eg. 1999 Smolt</t>
+  </si>
+  <si>
+    <t>UFID associated with a  sample. Optional</t>
+  </si>
+  <si>
+    <t>Eg. Fry/Parr/Smolt. Optional</t>
+  </si>
+  <si>
+    <t>Number of fish in group. Optional</t>
+  </si>
+  <si>
+    <t>Did the group get split, or did it move as a whole? Optional</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -297,8 +269,8 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
@@ -317,7 +289,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -345,13 +317,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -371,11 +382,26 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -659,11 +685,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:O71"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:RU71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="A4:C5"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,119 +706,665 @@
     <col min="15" max="15" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="2" spans="1:489" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="P2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="S2" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="T2" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:489" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="14"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="14"/>
+      <c r="AX3" s="14"/>
+      <c r="AY3" s="14"/>
+      <c r="AZ3" s="14"/>
+      <c r="BA3" s="14"/>
+      <c r="BB3" s="14"/>
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+      <c r="BE3" s="14"/>
+      <c r="BF3" s="14"/>
+      <c r="BG3" s="14"/>
+      <c r="BH3" s="14"/>
+      <c r="BI3" s="14"/>
+      <c r="BJ3" s="14"/>
+      <c r="BK3" s="14"/>
+      <c r="BL3" s="14"/>
+      <c r="BM3" s="14"/>
+      <c r="BN3" s="14"/>
+      <c r="BO3" s="14"/>
+      <c r="BP3" s="14"/>
+      <c r="BQ3" s="14"/>
+      <c r="BR3" s="14"/>
+      <c r="BS3" s="14"/>
+      <c r="BT3" s="14"/>
+      <c r="BU3" s="14"/>
+      <c r="BV3" s="14"/>
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="14"/>
+      <c r="BZ3" s="14"/>
+      <c r="CA3" s="14"/>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="14"/>
+      <c r="CD3" s="14"/>
+      <c r="CE3" s="14"/>
+      <c r="CF3" s="14"/>
+      <c r="CG3" s="14"/>
+      <c r="CH3" s="14"/>
+      <c r="CI3" s="14"/>
+      <c r="CJ3" s="14"/>
+      <c r="CK3" s="14"/>
+      <c r="CL3" s="14"/>
+      <c r="CM3" s="14"/>
+      <c r="CN3" s="14"/>
+      <c r="CO3" s="14"/>
+      <c r="CP3" s="14"/>
+      <c r="CQ3" s="14"/>
+      <c r="CR3" s="14"/>
+      <c r="CS3" s="14"/>
+      <c r="CT3" s="14"/>
+      <c r="CU3" s="14"/>
+      <c r="CV3" s="14"/>
+      <c r="CW3" s="14"/>
+      <c r="CX3" s="14"/>
+      <c r="CY3" s="14"/>
+      <c r="CZ3" s="14"/>
+      <c r="DA3" s="14"/>
+      <c r="DB3" s="14"/>
+      <c r="DC3" s="14"/>
+      <c r="DD3" s="14"/>
+      <c r="DE3" s="14"/>
+      <c r="DF3" s="14"/>
+      <c r="DG3" s="14"/>
+      <c r="DH3" s="14"/>
+      <c r="DI3" s="14"/>
+      <c r="DJ3" s="14"/>
+      <c r="DK3" s="14"/>
+      <c r="DL3" s="14"/>
+      <c r="DM3" s="14"/>
+      <c r="DN3" s="14"/>
+      <c r="DO3" s="14"/>
+      <c r="DP3" s="14"/>
+      <c r="DQ3" s="14"/>
+      <c r="DR3" s="14"/>
+      <c r="DS3" s="14"/>
+      <c r="DT3" s="14"/>
+      <c r="DU3" s="14"/>
+      <c r="DV3" s="14"/>
+      <c r="DW3" s="14"/>
+      <c r="DX3" s="14"/>
+      <c r="DY3" s="14"/>
+      <c r="DZ3" s="14"/>
+      <c r="EA3" s="14"/>
+      <c r="EB3" s="14"/>
+      <c r="EC3" s="14"/>
+      <c r="ED3" s="14"/>
+      <c r="EE3" s="14"/>
+      <c r="EF3" s="14"/>
+      <c r="EG3" s="14"/>
+      <c r="EH3" s="14"/>
+      <c r="EI3" s="14"/>
+      <c r="EJ3" s="14"/>
+      <c r="EK3" s="14"/>
+      <c r="EL3" s="14"/>
+      <c r="EM3" s="14"/>
+      <c r="EN3" s="14"/>
+      <c r="EO3" s="14"/>
+      <c r="EP3" s="14"/>
+      <c r="EQ3" s="14"/>
+      <c r="ER3" s="14"/>
+      <c r="ES3" s="14"/>
+      <c r="ET3" s="14"/>
+      <c r="EU3" s="14"/>
+      <c r="EV3" s="14"/>
+      <c r="EW3" s="14"/>
+      <c r="EX3" s="14"/>
+      <c r="EY3" s="14"/>
+      <c r="EZ3" s="14"/>
+      <c r="FA3" s="14"/>
+      <c r="FB3" s="14"/>
+      <c r="FC3" s="14"/>
+      <c r="FD3" s="14"/>
+      <c r="FE3" s="14"/>
+      <c r="FF3" s="14"/>
+      <c r="FG3" s="14"/>
+      <c r="FH3" s="14"/>
+      <c r="FI3" s="14"/>
+      <c r="FJ3" s="14"/>
+      <c r="FK3" s="14"/>
+      <c r="FL3" s="14"/>
+      <c r="FM3" s="14"/>
+      <c r="FN3" s="14"/>
+      <c r="FO3" s="14"/>
+      <c r="FP3" s="14"/>
+      <c r="FQ3" s="14"/>
+      <c r="FR3" s="14"/>
+      <c r="FS3" s="14"/>
+      <c r="FT3" s="14"/>
+      <c r="FU3" s="14"/>
+      <c r="FV3" s="14"/>
+      <c r="FW3" s="14"/>
+      <c r="FX3" s="14"/>
+      <c r="FY3" s="14"/>
+      <c r="FZ3" s="14"/>
+      <c r="GA3" s="14"/>
+      <c r="GB3" s="14"/>
+      <c r="GC3" s="14"/>
+      <c r="GD3" s="14"/>
+      <c r="GE3" s="14"/>
+      <c r="GF3" s="14"/>
+      <c r="GG3" s="14"/>
+      <c r="GH3" s="14"/>
+      <c r="GI3" s="14"/>
+      <c r="GJ3" s="14"/>
+      <c r="GK3" s="14"/>
+      <c r="GL3" s="14"/>
+      <c r="GM3" s="14"/>
+      <c r="GN3" s="14"/>
+      <c r="GO3" s="14"/>
+      <c r="GP3" s="14"/>
+      <c r="GQ3" s="14"/>
+      <c r="GR3" s="14"/>
+      <c r="GS3" s="14"/>
+      <c r="GT3" s="14"/>
+      <c r="GU3" s="14"/>
+      <c r="GV3" s="14"/>
+      <c r="GW3" s="14"/>
+      <c r="GX3" s="14"/>
+      <c r="GY3" s="14"/>
+      <c r="GZ3" s="14"/>
+      <c r="HA3" s="14"/>
+      <c r="HB3" s="14"/>
+      <c r="HC3" s="14"/>
+      <c r="HD3" s="14"/>
+      <c r="HE3" s="14"/>
+      <c r="HF3" s="14"/>
+      <c r="HG3" s="14"/>
+      <c r="HH3" s="14"/>
+      <c r="HI3" s="14"/>
+      <c r="HJ3" s="14"/>
+      <c r="HK3" s="14"/>
+      <c r="HL3" s="14"/>
+      <c r="HM3" s="14"/>
+      <c r="HN3" s="14"/>
+      <c r="HO3" s="14"/>
+      <c r="HP3" s="14"/>
+      <c r="HQ3" s="14"/>
+      <c r="HR3" s="14"/>
+      <c r="HS3" s="14"/>
+      <c r="HT3" s="14"/>
+      <c r="HU3" s="14"/>
+      <c r="HV3" s="14"/>
+      <c r="HW3" s="14"/>
+      <c r="HX3" s="14"/>
+      <c r="HY3" s="14"/>
+      <c r="HZ3" s="14"/>
+      <c r="IA3" s="14"/>
+      <c r="IB3" s="14"/>
+      <c r="IC3" s="14"/>
+      <c r="ID3" s="14"/>
+      <c r="IE3" s="14"/>
+      <c r="IF3" s="14"/>
+      <c r="IG3" s="14"/>
+      <c r="IH3" s="14"/>
+      <c r="II3" s="14"/>
+      <c r="IJ3" s="14"/>
+      <c r="IK3" s="14"/>
+      <c r="IL3" s="14"/>
+      <c r="IM3" s="14"/>
+      <c r="IN3" s="14"/>
+      <c r="IO3" s="14"/>
+      <c r="IP3" s="14"/>
+      <c r="IQ3" s="14"/>
+      <c r="IR3" s="14"/>
+      <c r="IS3" s="14"/>
+      <c r="IT3" s="14"/>
+      <c r="IU3" s="14"/>
+      <c r="IV3" s="14"/>
+      <c r="IW3" s="14"/>
+      <c r="IX3" s="14"/>
+      <c r="IY3" s="14"/>
+      <c r="IZ3" s="14"/>
+      <c r="JA3" s="14"/>
+      <c r="JB3" s="14"/>
+      <c r="JC3" s="14"/>
+      <c r="JD3" s="14"/>
+      <c r="JE3" s="14"/>
+      <c r="JF3" s="14"/>
+      <c r="JG3" s="14"/>
+      <c r="JH3" s="14"/>
+      <c r="JI3" s="14"/>
+      <c r="JJ3" s="14"/>
+      <c r="JK3" s="14"/>
+      <c r="JL3" s="14"/>
+      <c r="JM3" s="14"/>
+      <c r="JN3" s="14"/>
+      <c r="JO3" s="14"/>
+      <c r="JP3" s="14"/>
+      <c r="JQ3" s="14"/>
+      <c r="JR3" s="14"/>
+      <c r="JS3" s="14"/>
+      <c r="JT3" s="14"/>
+      <c r="JU3" s="14"/>
+      <c r="JV3" s="14"/>
+      <c r="JW3" s="14"/>
+      <c r="JX3" s="14"/>
+      <c r="JY3" s="14"/>
+      <c r="JZ3" s="14"/>
+      <c r="KA3" s="14"/>
+      <c r="KB3" s="14"/>
+      <c r="KC3" s="14"/>
+      <c r="KD3" s="14"/>
+      <c r="KE3" s="14"/>
+      <c r="KF3" s="14"/>
+      <c r="KG3" s="14"/>
+      <c r="KH3" s="14"/>
+      <c r="KI3" s="14"/>
+      <c r="KJ3" s="14"/>
+      <c r="KK3" s="14"/>
+      <c r="KL3" s="14"/>
+      <c r="KM3" s="14"/>
+      <c r="KN3" s="14"/>
+      <c r="KO3" s="14"/>
+      <c r="KP3" s="14"/>
+      <c r="KQ3" s="14"/>
+      <c r="KR3" s="14"/>
+      <c r="KS3" s="14"/>
+      <c r="KT3" s="14"/>
+      <c r="KU3" s="14"/>
+      <c r="KV3" s="14"/>
+      <c r="KW3" s="14"/>
+      <c r="KX3" s="14"/>
+      <c r="KY3" s="14"/>
+      <c r="KZ3" s="14"/>
+      <c r="LA3" s="14"/>
+      <c r="LB3" s="14"/>
+      <c r="LC3" s="14"/>
+      <c r="LD3" s="14"/>
+      <c r="LE3" s="14"/>
+      <c r="LF3" s="14"/>
+      <c r="LG3" s="14"/>
+      <c r="LH3" s="14"/>
+      <c r="LI3" s="14"/>
+      <c r="LJ3" s="14"/>
+      <c r="LK3" s="14"/>
+      <c r="LL3" s="14"/>
+      <c r="LM3" s="14"/>
+      <c r="LN3" s="14"/>
+      <c r="LO3" s="14"/>
+      <c r="LP3" s="14"/>
+      <c r="LQ3" s="14"/>
+      <c r="LR3" s="14"/>
+      <c r="LS3" s="14"/>
+      <c r="LT3" s="14"/>
+      <c r="LU3" s="14"/>
+      <c r="LV3" s="14"/>
+      <c r="LW3" s="14"/>
+      <c r="LX3" s="14"/>
+      <c r="LY3" s="14"/>
+      <c r="LZ3" s="14"/>
+      <c r="MA3" s="14"/>
+      <c r="MB3" s="14"/>
+      <c r="MC3" s="14"/>
+      <c r="MD3" s="14"/>
+      <c r="ME3" s="14"/>
+      <c r="MF3" s="14"/>
+      <c r="MG3" s="14"/>
+      <c r="MH3" s="14"/>
+      <c r="MI3" s="14"/>
+      <c r="MJ3" s="14"/>
+      <c r="MK3" s="14"/>
+      <c r="ML3" s="14"/>
+      <c r="MM3" s="14"/>
+      <c r="MN3" s="14"/>
+      <c r="MO3" s="14"/>
+      <c r="MP3" s="14"/>
+      <c r="MQ3" s="14"/>
+      <c r="MR3" s="14"/>
+      <c r="MS3" s="14"/>
+      <c r="MT3" s="14"/>
+      <c r="MU3" s="14"/>
+      <c r="MV3" s="14"/>
+      <c r="MW3" s="14"/>
+      <c r="MX3" s="14"/>
+      <c r="MY3" s="14"/>
+      <c r="MZ3" s="14"/>
+      <c r="NA3" s="14"/>
+      <c r="NB3" s="14"/>
+      <c r="NC3" s="14"/>
+      <c r="ND3" s="14"/>
+      <c r="NE3" s="14"/>
+      <c r="NF3" s="14"/>
+      <c r="NG3" s="14"/>
+      <c r="NH3" s="14"/>
+      <c r="NI3" s="14"/>
+      <c r="NJ3" s="14"/>
+      <c r="NK3" s="14"/>
+      <c r="NL3" s="14"/>
+      <c r="NM3" s="14"/>
+      <c r="NN3" s="14"/>
+      <c r="NO3" s="14"/>
+      <c r="NP3" s="14"/>
+      <c r="NQ3" s="14"/>
+      <c r="NR3" s="14"/>
+      <c r="NS3" s="14"/>
+      <c r="NT3" s="14"/>
+      <c r="NU3" s="14"/>
+      <c r="NV3" s="14"/>
+      <c r="NW3" s="14"/>
+      <c r="NX3" s="14"/>
+      <c r="NY3" s="14"/>
+      <c r="NZ3" s="14"/>
+      <c r="OA3" s="14"/>
+      <c r="OB3" s="14"/>
+      <c r="OC3" s="14"/>
+      <c r="OD3" s="14"/>
+      <c r="OE3" s="14"/>
+      <c r="OF3" s="14"/>
+      <c r="OG3" s="14"/>
+      <c r="OH3" s="14"/>
+      <c r="OI3" s="14"/>
+      <c r="OJ3" s="14"/>
+      <c r="OK3" s="14"/>
+      <c r="OL3" s="14"/>
+      <c r="OM3" s="14"/>
+      <c r="ON3" s="14"/>
+      <c r="OO3" s="14"/>
+      <c r="OP3" s="14"/>
+      <c r="OQ3" s="14"/>
+      <c r="OR3" s="14"/>
+      <c r="OS3" s="14"/>
+      <c r="OT3" s="14"/>
+      <c r="OU3" s="14"/>
+      <c r="OV3" s="14"/>
+      <c r="OW3" s="14"/>
+      <c r="OX3" s="14"/>
+      <c r="OY3" s="14"/>
+      <c r="OZ3" s="14"/>
+      <c r="PA3" s="14"/>
+      <c r="PB3" s="14"/>
+      <c r="PC3" s="14"/>
+      <c r="PD3" s="14"/>
+      <c r="PE3" s="14"/>
+      <c r="PF3" s="14"/>
+      <c r="PG3" s="14"/>
+      <c r="PH3" s="14"/>
+      <c r="PI3" s="14"/>
+      <c r="PJ3" s="14"/>
+      <c r="PK3" s="14"/>
+      <c r="PL3" s="14"/>
+      <c r="PM3" s="14"/>
+      <c r="PN3" s="14"/>
+      <c r="PO3" s="14"/>
+      <c r="PP3" s="14"/>
+      <c r="PQ3" s="14"/>
+      <c r="PR3" s="14"/>
+      <c r="PS3" s="14"/>
+      <c r="PT3" s="14"/>
+      <c r="PU3" s="14"/>
+      <c r="PV3" s="14"/>
+      <c r="PW3" s="14"/>
+      <c r="PX3" s="14"/>
+      <c r="PY3" s="14"/>
+      <c r="PZ3" s="14"/>
+      <c r="QA3" s="14"/>
+      <c r="QB3" s="14"/>
+      <c r="QC3" s="14"/>
+      <c r="QD3" s="14"/>
+      <c r="QE3" s="14"/>
+      <c r="QF3" s="14"/>
+      <c r="QG3" s="14"/>
+      <c r="QH3" s="14"/>
+      <c r="QI3" s="14"/>
+      <c r="QJ3" s="14"/>
+      <c r="QK3" s="14"/>
+      <c r="QL3" s="14"/>
+      <c r="QM3" s="14"/>
+      <c r="QN3" s="14"/>
+      <c r="QO3" s="14"/>
+      <c r="QP3" s="14"/>
+      <c r="QQ3" s="14"/>
+      <c r="QR3" s="14"/>
+      <c r="QS3" s="14"/>
+      <c r="QT3" s="14"/>
+      <c r="QU3" s="14"/>
+      <c r="QV3" s="14"/>
+      <c r="QW3" s="14"/>
+      <c r="QX3" s="14"/>
+      <c r="QY3" s="14"/>
+      <c r="QZ3" s="14"/>
+      <c r="RA3" s="14"/>
+      <c r="RB3" s="14"/>
+      <c r="RC3" s="14"/>
+      <c r="RD3" s="14"/>
+      <c r="RE3" s="14"/>
+      <c r="RF3" s="14"/>
+      <c r="RG3" s="14"/>
+      <c r="RH3" s="14"/>
+      <c r="RI3" s="14"/>
+      <c r="RJ3" s="14"/>
+      <c r="RK3" s="14"/>
+      <c r="RL3" s="14"/>
+      <c r="RM3" s="14"/>
+      <c r="RN3" s="14"/>
+      <c r="RO3" s="14"/>
+      <c r="RP3" s="14"/>
+      <c r="RQ3" s="14"/>
+      <c r="RR3" s="14"/>
+      <c r="RS3" s="14"/>
+      <c r="RT3" s="14"/>
+      <c r="RU3" s="14"/>
+    </row>
+    <row r="4" spans="1:489" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D4" s="4"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:489" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:489" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="4"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="1"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C8" s="2"/>
       <c r="D8" s="1"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C9" s="2"/>
       <c r="D9" s="1"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C10" s="2"/>
       <c r="D10" s="1"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C11" s="2"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C13" s="2"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C14" s="2"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C15" s="2"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:489" x14ac:dyDescent="0.25">
       <c r="C16" s="2"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -1079,11 +1651,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:S21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A2:RU21"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,75 +1671,620 @@
     <col min="19" max="19" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="D2" s="2"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
+    <row r="2" spans="1:489" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K2" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="N2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="P3" s="5" t="s">
+      <c r="P2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="R3" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="U2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="W2" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="X2" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:489" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="R3" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="S3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="V3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14"/>
+      <c r="AA3" s="14"/>
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14"/>
+      <c r="AD3" s="14"/>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14"/>
+      <c r="AG3" s="14"/>
+      <c r="AH3" s="14"/>
+      <c r="AI3" s="14"/>
+      <c r="AJ3" s="14"/>
+      <c r="AK3" s="14"/>
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="14"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
+      <c r="AP3" s="14"/>
+      <c r="AQ3" s="14"/>
+      <c r="AR3" s="14"/>
+      <c r="AS3" s="14"/>
+      <c r="AT3" s="14"/>
+      <c r="AU3" s="14"/>
+      <c r="AV3" s="14"/>
+      <c r="AW3" s="14"/>
+      <c r="AX3" s="14"/>
+      <c r="AY3" s="14"/>
+      <c r="AZ3" s="14"/>
+      <c r="BA3" s="14"/>
+      <c r="BB3" s="14"/>
+      <c r="BC3" s="14"/>
+      <c r="BD3" s="14"/>
+      <c r="BE3" s="14"/>
+      <c r="BF3" s="14"/>
+      <c r="BG3" s="14"/>
+      <c r="BH3" s="14"/>
+      <c r="BI3" s="14"/>
+      <c r="BJ3" s="14"/>
+      <c r="BK3" s="14"/>
+      <c r="BL3" s="14"/>
+      <c r="BM3" s="14"/>
+      <c r="BN3" s="14"/>
+      <c r="BO3" s="14"/>
+      <c r="BP3" s="14"/>
+      <c r="BQ3" s="14"/>
+      <c r="BR3" s="14"/>
+      <c r="BS3" s="14"/>
+      <c r="BT3" s="14"/>
+      <c r="BU3" s="14"/>
+      <c r="BV3" s="14"/>
+      <c r="BW3" s="14"/>
+      <c r="BX3" s="14"/>
+      <c r="BY3" s="14"/>
+      <c r="BZ3" s="14"/>
+      <c r="CA3" s="14"/>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="14"/>
+      <c r="CD3" s="14"/>
+      <c r="CE3" s="14"/>
+      <c r="CF3" s="14"/>
+      <c r="CG3" s="14"/>
+      <c r="CH3" s="14"/>
+      <c r="CI3" s="14"/>
+      <c r="CJ3" s="14"/>
+      <c r="CK3" s="14"/>
+      <c r="CL3" s="14"/>
+      <c r="CM3" s="14"/>
+      <c r="CN3" s="14"/>
+      <c r="CO3" s="14"/>
+      <c r="CP3" s="14"/>
+      <c r="CQ3" s="14"/>
+      <c r="CR3" s="14"/>
+      <c r="CS3" s="14"/>
+      <c r="CT3" s="14"/>
+      <c r="CU3" s="14"/>
+      <c r="CV3" s="14"/>
+      <c r="CW3" s="14"/>
+      <c r="CX3" s="14"/>
+      <c r="CY3" s="14"/>
+      <c r="CZ3" s="14"/>
+      <c r="DA3" s="14"/>
+      <c r="DB3" s="14"/>
+      <c r="DC3" s="14"/>
+      <c r="DD3" s="14"/>
+      <c r="DE3" s="14"/>
+      <c r="DF3" s="14"/>
+      <c r="DG3" s="14"/>
+      <c r="DH3" s="14"/>
+      <c r="DI3" s="14"/>
+      <c r="DJ3" s="14"/>
+      <c r="DK3" s="14"/>
+      <c r="DL3" s="14"/>
+      <c r="DM3" s="14"/>
+      <c r="DN3" s="14"/>
+      <c r="DO3" s="14"/>
+      <c r="DP3" s="14"/>
+      <c r="DQ3" s="14"/>
+      <c r="DR3" s="14"/>
+      <c r="DS3" s="14"/>
+      <c r="DT3" s="14"/>
+      <c r="DU3" s="14"/>
+      <c r="DV3" s="14"/>
+      <c r="DW3" s="14"/>
+      <c r="DX3" s="14"/>
+      <c r="DY3" s="14"/>
+      <c r="DZ3" s="14"/>
+      <c r="EA3" s="14"/>
+      <c r="EB3" s="14"/>
+      <c r="EC3" s="14"/>
+      <c r="ED3" s="14"/>
+      <c r="EE3" s="14"/>
+      <c r="EF3" s="14"/>
+      <c r="EG3" s="14"/>
+      <c r="EH3" s="14"/>
+      <c r="EI3" s="14"/>
+      <c r="EJ3" s="14"/>
+      <c r="EK3" s="14"/>
+      <c r="EL3" s="14"/>
+      <c r="EM3" s="14"/>
+      <c r="EN3" s="14"/>
+      <c r="EO3" s="14"/>
+      <c r="EP3" s="14"/>
+      <c r="EQ3" s="14"/>
+      <c r="ER3" s="14"/>
+      <c r="ES3" s="14"/>
+      <c r="ET3" s="14"/>
+      <c r="EU3" s="14"/>
+      <c r="EV3" s="14"/>
+      <c r="EW3" s="14"/>
+      <c r="EX3" s="14"/>
+      <c r="EY3" s="14"/>
+      <c r="EZ3" s="14"/>
+      <c r="FA3" s="14"/>
+      <c r="FB3" s="14"/>
+      <c r="FC3" s="14"/>
+      <c r="FD3" s="14"/>
+      <c r="FE3" s="14"/>
+      <c r="FF3" s="14"/>
+      <c r="FG3" s="14"/>
+      <c r="FH3" s="14"/>
+      <c r="FI3" s="14"/>
+      <c r="FJ3" s="14"/>
+      <c r="FK3" s="14"/>
+      <c r="FL3" s="14"/>
+      <c r="FM3" s="14"/>
+      <c r="FN3" s="14"/>
+      <c r="FO3" s="14"/>
+      <c r="FP3" s="14"/>
+      <c r="FQ3" s="14"/>
+      <c r="FR3" s="14"/>
+      <c r="FS3" s="14"/>
+      <c r="FT3" s="14"/>
+      <c r="FU3" s="14"/>
+      <c r="FV3" s="14"/>
+      <c r="FW3" s="14"/>
+      <c r="FX3" s="14"/>
+      <c r="FY3" s="14"/>
+      <c r="FZ3" s="14"/>
+      <c r="GA3" s="14"/>
+      <c r="GB3" s="14"/>
+      <c r="GC3" s="14"/>
+      <c r="GD3" s="14"/>
+      <c r="GE3" s="14"/>
+      <c r="GF3" s="14"/>
+      <c r="GG3" s="14"/>
+      <c r="GH3" s="14"/>
+      <c r="GI3" s="14"/>
+      <c r="GJ3" s="14"/>
+      <c r="GK3" s="14"/>
+      <c r="GL3" s="14"/>
+      <c r="GM3" s="14"/>
+      <c r="GN3" s="14"/>
+      <c r="GO3" s="14"/>
+      <c r="GP3" s="14"/>
+      <c r="GQ3" s="14"/>
+      <c r="GR3" s="14"/>
+      <c r="GS3" s="14"/>
+      <c r="GT3" s="14"/>
+      <c r="GU3" s="14"/>
+      <c r="GV3" s="14"/>
+      <c r="GW3" s="14"/>
+      <c r="GX3" s="14"/>
+      <c r="GY3" s="14"/>
+      <c r="GZ3" s="14"/>
+      <c r="HA3" s="14"/>
+      <c r="HB3" s="14"/>
+      <c r="HC3" s="14"/>
+      <c r="HD3" s="14"/>
+      <c r="HE3" s="14"/>
+      <c r="HF3" s="14"/>
+      <c r="HG3" s="14"/>
+      <c r="HH3" s="14"/>
+      <c r="HI3" s="14"/>
+      <c r="HJ3" s="14"/>
+      <c r="HK3" s="14"/>
+      <c r="HL3" s="14"/>
+      <c r="HM3" s="14"/>
+      <c r="HN3" s="14"/>
+      <c r="HO3" s="14"/>
+      <c r="HP3" s="14"/>
+      <c r="HQ3" s="14"/>
+      <c r="HR3" s="14"/>
+      <c r="HS3" s="14"/>
+      <c r="HT3" s="14"/>
+      <c r="HU3" s="14"/>
+      <c r="HV3" s="14"/>
+      <c r="HW3" s="14"/>
+      <c r="HX3" s="14"/>
+      <c r="HY3" s="14"/>
+      <c r="HZ3" s="14"/>
+      <c r="IA3" s="14"/>
+      <c r="IB3" s="14"/>
+      <c r="IC3" s="14"/>
+      <c r="ID3" s="14"/>
+      <c r="IE3" s="14"/>
+      <c r="IF3" s="14"/>
+      <c r="IG3" s="14"/>
+      <c r="IH3" s="14"/>
+      <c r="II3" s="14"/>
+      <c r="IJ3" s="14"/>
+      <c r="IK3" s="14"/>
+      <c r="IL3" s="14"/>
+      <c r="IM3" s="14"/>
+      <c r="IN3" s="14"/>
+      <c r="IO3" s="14"/>
+      <c r="IP3" s="14"/>
+      <c r="IQ3" s="14"/>
+      <c r="IR3" s="14"/>
+      <c r="IS3" s="14"/>
+      <c r="IT3" s="14"/>
+      <c r="IU3" s="14"/>
+      <c r="IV3" s="14"/>
+      <c r="IW3" s="14"/>
+      <c r="IX3" s="14"/>
+      <c r="IY3" s="14"/>
+      <c r="IZ3" s="14"/>
+      <c r="JA3" s="14"/>
+      <c r="JB3" s="14"/>
+      <c r="JC3" s="14"/>
+      <c r="JD3" s="14"/>
+      <c r="JE3" s="14"/>
+      <c r="JF3" s="14"/>
+      <c r="JG3" s="14"/>
+      <c r="JH3" s="14"/>
+      <c r="JI3" s="14"/>
+      <c r="JJ3" s="14"/>
+      <c r="JK3" s="14"/>
+      <c r="JL3" s="14"/>
+      <c r="JM3" s="14"/>
+      <c r="JN3" s="14"/>
+      <c r="JO3" s="14"/>
+      <c r="JP3" s="14"/>
+      <c r="JQ3" s="14"/>
+      <c r="JR3" s="14"/>
+      <c r="JS3" s="14"/>
+      <c r="JT3" s="14"/>
+      <c r="JU3" s="14"/>
+      <c r="JV3" s="14"/>
+      <c r="JW3" s="14"/>
+      <c r="JX3" s="14"/>
+      <c r="JY3" s="14"/>
+      <c r="JZ3" s="14"/>
+      <c r="KA3" s="14"/>
+      <c r="KB3" s="14"/>
+      <c r="KC3" s="14"/>
+      <c r="KD3" s="14"/>
+      <c r="KE3" s="14"/>
+      <c r="KF3" s="14"/>
+      <c r="KG3" s="14"/>
+      <c r="KH3" s="14"/>
+      <c r="KI3" s="14"/>
+      <c r="KJ3" s="14"/>
+      <c r="KK3" s="14"/>
+      <c r="KL3" s="14"/>
+      <c r="KM3" s="14"/>
+      <c r="KN3" s="14"/>
+      <c r="KO3" s="14"/>
+      <c r="KP3" s="14"/>
+      <c r="KQ3" s="14"/>
+      <c r="KR3" s="14"/>
+      <c r="KS3" s="14"/>
+      <c r="KT3" s="14"/>
+      <c r="KU3" s="14"/>
+      <c r="KV3" s="14"/>
+      <c r="KW3" s="14"/>
+      <c r="KX3" s="14"/>
+      <c r="KY3" s="14"/>
+      <c r="KZ3" s="14"/>
+      <c r="LA3" s="14"/>
+      <c r="LB3" s="14"/>
+      <c r="LC3" s="14"/>
+      <c r="LD3" s="14"/>
+      <c r="LE3" s="14"/>
+      <c r="LF3" s="14"/>
+      <c r="LG3" s="14"/>
+      <c r="LH3" s="14"/>
+      <c r="LI3" s="14"/>
+      <c r="LJ3" s="14"/>
+      <c r="LK3" s="14"/>
+      <c r="LL3" s="14"/>
+      <c r="LM3" s="14"/>
+      <c r="LN3" s="14"/>
+      <c r="LO3" s="14"/>
+      <c r="LP3" s="14"/>
+      <c r="LQ3" s="14"/>
+      <c r="LR3" s="14"/>
+      <c r="LS3" s="14"/>
+      <c r="LT3" s="14"/>
+      <c r="LU3" s="14"/>
+      <c r="LV3" s="14"/>
+      <c r="LW3" s="14"/>
+      <c r="LX3" s="14"/>
+      <c r="LY3" s="14"/>
+      <c r="LZ3" s="14"/>
+      <c r="MA3" s="14"/>
+      <c r="MB3" s="14"/>
+      <c r="MC3" s="14"/>
+      <c r="MD3" s="14"/>
+      <c r="ME3" s="14"/>
+      <c r="MF3" s="14"/>
+      <c r="MG3" s="14"/>
+      <c r="MH3" s="14"/>
+      <c r="MI3" s="14"/>
+      <c r="MJ3" s="14"/>
+      <c r="MK3" s="14"/>
+      <c r="ML3" s="14"/>
+      <c r="MM3" s="14"/>
+      <c r="MN3" s="14"/>
+      <c r="MO3" s="14"/>
+      <c r="MP3" s="14"/>
+      <c r="MQ3" s="14"/>
+      <c r="MR3" s="14"/>
+      <c r="MS3" s="14"/>
+      <c r="MT3" s="14"/>
+      <c r="MU3" s="14"/>
+      <c r="MV3" s="14"/>
+      <c r="MW3" s="14"/>
+      <c r="MX3" s="14"/>
+      <c r="MY3" s="14"/>
+      <c r="MZ3" s="14"/>
+      <c r="NA3" s="14"/>
+      <c r="NB3" s="14"/>
+      <c r="NC3" s="14"/>
+      <c r="ND3" s="14"/>
+      <c r="NE3" s="14"/>
+      <c r="NF3" s="14"/>
+      <c r="NG3" s="14"/>
+      <c r="NH3" s="14"/>
+      <c r="NI3" s="14"/>
+      <c r="NJ3" s="14"/>
+      <c r="NK3" s="14"/>
+      <c r="NL3" s="14"/>
+      <c r="NM3" s="14"/>
+      <c r="NN3" s="14"/>
+      <c r="NO3" s="14"/>
+      <c r="NP3" s="14"/>
+      <c r="NQ3" s="14"/>
+      <c r="NR3" s="14"/>
+      <c r="NS3" s="14"/>
+      <c r="NT3" s="14"/>
+      <c r="NU3" s="14"/>
+      <c r="NV3" s="14"/>
+      <c r="NW3" s="14"/>
+      <c r="NX3" s="14"/>
+      <c r="NY3" s="14"/>
+      <c r="NZ3" s="14"/>
+      <c r="OA3" s="14"/>
+      <c r="OB3" s="14"/>
+      <c r="OC3" s="14"/>
+      <c r="OD3" s="14"/>
+      <c r="OE3" s="14"/>
+      <c r="OF3" s="14"/>
+      <c r="OG3" s="14"/>
+      <c r="OH3" s="14"/>
+      <c r="OI3" s="14"/>
+      <c r="OJ3" s="14"/>
+      <c r="OK3" s="14"/>
+      <c r="OL3" s="14"/>
+      <c r="OM3" s="14"/>
+      <c r="ON3" s="14"/>
+      <c r="OO3" s="14"/>
+      <c r="OP3" s="14"/>
+      <c r="OQ3" s="14"/>
+      <c r="OR3" s="14"/>
+      <c r="OS3" s="14"/>
+      <c r="OT3" s="14"/>
+      <c r="OU3" s="14"/>
+      <c r="OV3" s="14"/>
+      <c r="OW3" s="14"/>
+      <c r="OX3" s="14"/>
+      <c r="OY3" s="14"/>
+      <c r="OZ3" s="14"/>
+      <c r="PA3" s="14"/>
+      <c r="PB3" s="14"/>
+      <c r="PC3" s="14"/>
+      <c r="PD3" s="14"/>
+      <c r="PE3" s="14"/>
+      <c r="PF3" s="14"/>
+      <c r="PG3" s="14"/>
+      <c r="PH3" s="14"/>
+      <c r="PI3" s="14"/>
+      <c r="PJ3" s="14"/>
+      <c r="PK3" s="14"/>
+      <c r="PL3" s="14"/>
+      <c r="PM3" s="14"/>
+      <c r="PN3" s="14"/>
+      <c r="PO3" s="14"/>
+      <c r="PP3" s="14"/>
+      <c r="PQ3" s="14"/>
+      <c r="PR3" s="14"/>
+      <c r="PS3" s="14"/>
+      <c r="PT3" s="14"/>
+      <c r="PU3" s="14"/>
+      <c r="PV3" s="14"/>
+      <c r="PW3" s="14"/>
+      <c r="PX3" s="14"/>
+      <c r="PY3" s="14"/>
+      <c r="PZ3" s="14"/>
+      <c r="QA3" s="14"/>
+      <c r="QB3" s="14"/>
+      <c r="QC3" s="14"/>
+      <c r="QD3" s="14"/>
+      <c r="QE3" s="14"/>
+      <c r="QF3" s="14"/>
+      <c r="QG3" s="14"/>
+      <c r="QH3" s="14"/>
+      <c r="QI3" s="14"/>
+      <c r="QJ3" s="14"/>
+      <c r="QK3" s="14"/>
+      <c r="QL3" s="14"/>
+      <c r="QM3" s="14"/>
+      <c r="QN3" s="14"/>
+      <c r="QO3" s="14"/>
+      <c r="QP3" s="14"/>
+      <c r="QQ3" s="14"/>
+      <c r="QR3" s="14"/>
+      <c r="QS3" s="14"/>
+      <c r="QT3" s="14"/>
+      <c r="QU3" s="14"/>
+      <c r="QV3" s="14"/>
+      <c r="QW3" s="14"/>
+      <c r="QX3" s="14"/>
+      <c r="QY3" s="14"/>
+      <c r="QZ3" s="14"/>
+      <c r="RA3" s="14"/>
+      <c r="RB3" s="14"/>
+      <c r="RC3" s="14"/>
+      <c r="RD3" s="14"/>
+      <c r="RE3" s="14"/>
+      <c r="RF3" s="14"/>
+      <c r="RG3" s="14"/>
+      <c r="RH3" s="14"/>
+      <c r="RI3" s="14"/>
+      <c r="RJ3" s="14"/>
+      <c r="RK3" s="14"/>
+      <c r="RL3" s="14"/>
+      <c r="RM3" s="14"/>
+      <c r="RN3" s="14"/>
+      <c r="RO3" s="14"/>
+      <c r="RP3" s="14"/>
+      <c r="RQ3" s="14"/>
+      <c r="RR3" s="14"/>
+      <c r="RS3" s="14"/>
+      <c r="RT3" s="14"/>
+      <c r="RU3" s="14"/>
+    </row>
+    <row r="4" spans="1:489" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1204,53 +2321,53 @@
       <c r="N4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="S4" t="s">
+      <c r="W4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="L10" s="3"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="L11" s="3"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="L12" s="3"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="L13" s="3"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="L15" s="3"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:489" x14ac:dyDescent="0.25">
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1299,11 +2416,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1316,7 +2433,7 @@
     <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D1" s="2"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -1324,51 +2441,101 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:14" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+    <row r="2" spans="1:15" s="8" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="L2" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="O2" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="8" customFormat="1" ht="127.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -1402,7 +2569,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="D5" s="2"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1412,6 +2579,5 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>